<commit_message>
Tested multiple lab sessions for a course
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/CAES-2020-Sem1-Wvl/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/CAES-2020-Sem1-Wvl/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\CAES-2020-Sem1-Wvl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA04263-885E-416E-9E50-E79109FF2AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557C2B1-ADA9-4574-91EB-04E478B66148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>